<commit_message>
Update Math standard with dependencies
</commit_message>
<xml_diff>
--- a/Sonstiges/CCSS-Math.xlsx
+++ b/Sonstiges/CCSS-Math.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\07 Dokumente\Duales Studium\DHBW\5. Semester\00 Studienarbeit\NoRPG-docs\Sonstiges\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035"/>
   </bookViews>
@@ -429,9 +434,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Location in NoRPG</t>
-  </si>
-  <si>
     <t>addition and subtraction within 20</t>
   </si>
   <si>
@@ -583,9 +585,6 @@
     <t>Add and subtract within 1000</t>
   </si>
   <si>
-    <t>Mentally add 10 or 100 to a given number 100-900, and mentally subtract 10 or 100 from a given number 100-900.</t>
-  </si>
-  <si>
     <t>Explain why addition and subtraction strategies work, using place value and the properties of operations</t>
   </si>
   <si>
@@ -1221,11 +1220,17 @@
   <si>
     <t>Classify two-dimensional figures in a hierarchy based on properties.</t>
   </si>
+  <si>
+    <t>Mentally add 10 or 100 to a given number 100-900, and mentally subtract 10 or 100 from a given number 100-900</t>
+  </si>
+  <si>
+    <t>Abhängigkeiten</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1259,7 +1264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1289,7 +1294,48 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -1299,21 +1345,12 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1326,7 +1363,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -1338,13 +1375,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1356,23 +1408,38 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1384,10 +1451,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1396,25 +1463,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -1426,101 +1478,15 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1554,83 +1520,195 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1639,14 +1717,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1684,9 +1765,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1719,9 +1800,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1754,9 +1852,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1932,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,1476 +2061,1516 @@
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
+        <v>1</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="20" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="19"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="19"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="23"/>
+      <c r="B21" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" s="10"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
+      <c r="B23" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29"/>
+      <c r="B24" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="20" t="s">
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="22">
+        <v>2</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E24" s="19"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>2</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="22" t="s">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="19"/>
+    </row>
+    <row r="28" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="23"/>
+      <c r="B28" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="E28" s="10"/>
+      <c r="E28" s="21"/>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E29" s="17"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="18"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="19"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+      <c r="B35" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="23"/>
+      <c r="B37" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="30"/>
+      <c r="D37" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E37" s="10"/>
+      <c r="E37" s="21"/>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" s="17"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+      <c r="B39" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E39" s="20"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="5" t="s">
+      <c r="E40" s="20"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="11"/>
+      <c r="D41" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="5" t="s">
+      <c r="E41" s="18"/>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
+      <c r="B42" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="5" t="s">
+      <c r="E42" s="19"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
+      <c r="B43" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="5" t="s">
+      <c r="E43" s="18"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="D44" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="5" t="s">
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="5" t="s">
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="D46" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="5" t="s">
+      <c r="E46" s="19"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="23"/>
+      <c r="B47" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
-      <c r="B47" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="E47" s="10"/>
+      <c r="E47" s="21"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="E48" s="17"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="29"/>
+      <c r="B50" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="E48" s="10"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
-      <c r="B49" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="5" t="s">
+      <c r="E50" s="21"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="22">
+        <v>3</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
-      <c r="B50" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="20" t="s">
+      <c r="E51" s="17"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+      <c r="B52" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E50" s="19"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="6">
-        <v>3</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D51" s="22" t="s">
+      <c r="E52" s="20"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+      <c r="B53" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E51" s="8"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="5" t="s">
+      <c r="E53" s="20"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+      <c r="B54" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="11"/>
+      <c r="D54" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
-      <c r="B53" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="5" t="s">
+      <c r="E54" s="18"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="B55" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="D55" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E53" s="10"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="5" t="s">
+      <c r="E55" s="19"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
+      <c r="B56" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
-      <c r="B55" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="5" t="s">
+      <c r="E56" s="18"/>
+    </row>
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+      <c r="B57" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="11"/>
+      <c r="D57" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
-      <c r="B56" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="5" t="s">
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="11"/>
+      <c r="D58" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E56" s="10"/>
-    </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="9"/>
-      <c r="B57" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="5" t="s">
+      <c r="E58" s="19"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="23"/>
+      <c r="B59" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="12"/>
+      <c r="D59" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="E57" s="10"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
-      <c r="B58" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="E58" s="10"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="9"/>
-      <c r="B59" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E59" s="10"/>
+      <c r="E59" s="21"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
+      <c r="A60" s="23"/>
       <c r="B60" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="E60" s="17"/>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+      <c r="B61" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E61" s="20"/>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="23"/>
+      <c r="B62" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="12"/>
+      <c r="D62" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="E60" s="10"/>
-    </row>
-    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="9"/>
-      <c r="B61" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="E61" s="10"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
-      <c r="B62" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="E62" s="10"/>
+      <c r="E62" s="21"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="9"/>
+      <c r="A63" s="23"/>
       <c r="B63" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E63" s="17"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+      <c r="B64" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E64" s="20"/>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="23"/>
+      <c r="B65" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" s="12"/>
+      <c r="D65" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="E63" s="10"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="9"/>
-      <c r="B64" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="E64" s="10"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="9"/>
-      <c r="B65" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E65" s="10"/>
+      <c r="E65" s="21"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
+      <c r="A66" s="23"/>
       <c r="B66" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E66" s="17"/>
+    </row>
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="23"/>
+      <c r="B67" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" s="11"/>
+      <c r="D67" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E67" s="18"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="23"/>
+      <c r="B68" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E66" s="10"/>
-    </row>
-    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
-      <c r="B67" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="5" t="s">
+      <c r="E68" s="19"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="23"/>
+      <c r="B69" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E67" s="10"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="9"/>
-      <c r="B68" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="5" t="s">
+      <c r="E69" s="18"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="23"/>
+      <c r="B70" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="11"/>
+      <c r="D70" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E68" s="10"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="9"/>
-      <c r="B69" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" s="3"/>
-      <c r="D69" s="5" t="s">
+      <c r="E70" s="19"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="23"/>
+      <c r="B71" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="11"/>
+      <c r="D71" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E69" s="10"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
-      <c r="B70" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="5" t="s">
+      <c r="E71" s="20"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="23"/>
+      <c r="B72" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" s="11"/>
+      <c r="D72" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E70" s="10"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="9"/>
-      <c r="B71" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="5" t="s">
+      <c r="E72" s="18"/>
+    </row>
+    <row r="73" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="23"/>
+      <c r="B73" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" s="12"/>
+      <c r="D73" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="E71" s="10"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="9"/>
-      <c r="B72" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E72" s="10"/>
-    </row>
-    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
-      <c r="B73" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E73" s="10"/>
+      <c r="E73" s="4"/>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
+      <c r="A74" s="23"/>
       <c r="B74" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="E74" s="17"/>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="29"/>
+      <c r="B75" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="E75" s="21"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="22">
+        <v>4</v>
+      </c>
+      <c r="B76" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D76" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E74" s="10"/>
-    </row>
-    <row r="75" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="18"/>
-      <c r="B75" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="20" t="s">
+      <c r="E76" s="17"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="23"/>
+      <c r="B77" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E75" s="19"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="6">
-        <v>4</v>
-      </c>
-      <c r="B76" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D76" s="22" t="s">
+      <c r="E77" s="20"/>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="23"/>
+      <c r="B78" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78" s="11"/>
+      <c r="D78" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E76" s="8"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="9"/>
-      <c r="B77" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" s="3"/>
-      <c r="D77" s="5" t="s">
+      <c r="E78" s="18"/>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="23"/>
+      <c r="B79" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C79" s="11"/>
+      <c r="D79" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E77" s="10"/>
-    </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="9"/>
-      <c r="B78" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="5" t="s">
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="23"/>
+      <c r="B80" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C80" s="12"/>
+      <c r="D80" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="E78" s="10"/>
-    </row>
-    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="9"/>
-      <c r="B79" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C79" s="3"/>
-      <c r="D79" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E79" s="10"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="9"/>
-      <c r="B80" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E80" s="10"/>
+      <c r="E80" s="4"/>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="9"/>
+      <c r="A81" s="23"/>
       <c r="B81" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="E81" s="17"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="23"/>
+      <c r="B82" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C82" s="11"/>
+      <c r="D82" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E82" s="20"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="23"/>
+      <c r="B83" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E81" s="10"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
-      <c r="B82" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="5" t="s">
+      <c r="E83" s="18"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="23"/>
+      <c r="B84" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84" s="11"/>
+      <c r="D84" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E82" s="10"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="9"/>
-      <c r="B83" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C83" s="3"/>
-      <c r="D83" s="5" t="s">
+      <c r="E84" s="19"/>
+    </row>
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="23"/>
+      <c r="B85" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="11"/>
+      <c r="D85" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E83" s="10"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
-      <c r="B84" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="5" t="s">
+      <c r="E85" s="20"/>
+    </row>
+    <row r="86" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="23"/>
+      <c r="B86" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C86" s="12"/>
+      <c r="D86" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="E84" s="10"/>
-    </row>
-    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="9"/>
-      <c r="B85" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C85" s="3"/>
-      <c r="D85" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E85" s="10"/>
-    </row>
-    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
-      <c r="B86" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C86" s="4"/>
-      <c r="D86" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E86" s="10"/>
+      <c r="E86" s="21"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
+      <c r="A87" s="23"/>
       <c r="B87" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="E87" s="17"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="23"/>
+      <c r="B88" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C88" s="11"/>
+      <c r="D88" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E88" s="18"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="23"/>
+      <c r="B89" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C89" s="11"/>
+      <c r="D89" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E87" s="10"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="9"/>
-      <c r="B88" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C88" s="3"/>
-      <c r="D88" s="5" t="s">
+      <c r="E89" s="19"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="23"/>
+      <c r="B90" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C90" s="11"/>
+      <c r="D90" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E88" s="10"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
-      <c r="B89" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C89" s="3"/>
-      <c r="D89" s="5" t="s">
+      <c r="E90" s="18"/>
+    </row>
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="23"/>
+      <c r="B91" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C91" s="11"/>
+      <c r="D91" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E89" s="10"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
-      <c r="B90" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="5" t="s">
+      <c r="E91" s="19"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="23"/>
+      <c r="B92" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" s="11"/>
+      <c r="D92" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E90" s="10"/>
-    </row>
-    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="9"/>
-      <c r="B91" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C91" s="3"/>
-      <c r="D91" s="5" t="s">
+      <c r="E92" s="20"/>
+    </row>
+    <row r="93" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="23"/>
+      <c r="B93" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" s="12"/>
+      <c r="D93" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="E91" s="10"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
-      <c r="B92" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C92" s="3"/>
-      <c r="D92" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E92" s="10"/>
-    </row>
-    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="9"/>
-      <c r="B93" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C93" s="4"/>
-      <c r="D93" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E93" s="10"/>
+      <c r="E93" s="21"/>
     </row>
     <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="9"/>
+      <c r="A94" s="23"/>
       <c r="B94" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="E94" s="17"/>
+    </row>
+    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="23"/>
+      <c r="B95" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C95" s="11"/>
+      <c r="D95" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E95" s="20"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="23"/>
+      <c r="B96" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" s="11"/>
+      <c r="D96" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E94" s="10"/>
-    </row>
-    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="9"/>
-      <c r="B95" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C95" s="3"/>
-      <c r="D95" s="5" t="s">
+      <c r="E96" s="18"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="23"/>
+      <c r="B97" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C97" s="11"/>
+      <c r="D97" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E95" s="10"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="9"/>
-      <c r="B96" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C96" s="3"/>
-      <c r="D96" s="5" t="s">
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="23"/>
+      <c r="B98" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C98" s="11"/>
+      <c r="D98" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E96" s="10"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="9"/>
-      <c r="B97" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C97" s="3"/>
-      <c r="D97" s="5" t="s">
+      <c r="E98" s="19"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="23"/>
+      <c r="B99" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C99" s="11"/>
+      <c r="D99" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E97" s="10"/>
-    </row>
-    <row r="98" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="9"/>
-      <c r="B98" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C98" s="3"/>
-      <c r="D98" s="5" t="s">
+      <c r="E99" s="20"/>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="23"/>
+      <c r="B100" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C100" s="12"/>
+      <c r="D100" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E98" s="10"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="9"/>
-      <c r="B99" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C99" s="3"/>
-      <c r="D99" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="E99" s="10"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="9"/>
-      <c r="B100" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C100" s="4"/>
-      <c r="D100" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E100" s="10"/>
+      <c r="E100" s="21"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="9"/>
+      <c r="A101" s="23"/>
       <c r="B101" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="E101" s="17"/>
+    </row>
+    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="23"/>
+      <c r="B102" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C102" s="11"/>
+      <c r="D102" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E102" s="20"/>
+    </row>
+    <row r="103" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="29"/>
+      <c r="B103" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C103" s="12"/>
+      <c r="D103" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="E101" s="10"/>
-    </row>
-    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="9"/>
-      <c r="B102" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C102" s="3"/>
-      <c r="D102" s="5" t="s">
+      <c r="E103" s="21"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="22">
+        <v>5</v>
+      </c>
+      <c r="B104" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D104" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="E102" s="10"/>
-    </row>
-    <row r="103" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="18"/>
-      <c r="B103" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C103" s="3"/>
-      <c r="D103" s="20" t="s">
+      <c r="E104" s="17"/>
+    </row>
+    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="23"/>
+      <c r="B105" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E103" s="19"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="6">
-        <v>5</v>
-      </c>
-      <c r="B104" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D104" s="22" t="s">
+      <c r="E105" s="18"/>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="23"/>
+      <c r="B106" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C106" s="12"/>
+      <c r="D106" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="E104" s="8"/>
-    </row>
-    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="9"/>
-      <c r="B105" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C105" s="3"/>
-      <c r="D105" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E105" s="10"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="9"/>
-      <c r="B106" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C106" s="4"/>
-      <c r="D106" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="E106" s="10"/>
+      <c r="E106" s="4"/>
     </row>
     <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="9"/>
+      <c r="A107" s="23"/>
       <c r="B107" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="D107" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="E107" s="17"/>
+    </row>
+    <row r="108" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="23"/>
+      <c r="B108" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C108" s="11"/>
+      <c r="D108" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E108" s="20"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="23"/>
+      <c r="B109" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C109" s="11"/>
+      <c r="D109" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E107" s="10"/>
-    </row>
-    <row r="108" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="9"/>
-      <c r="B108" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C108" s="3"/>
-      <c r="D108" s="5" t="s">
+      <c r="E109" s="20"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="23"/>
+      <c r="B110" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C110" s="11"/>
+      <c r="D110" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E108" s="10"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="9"/>
-      <c r="B109" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C109" s="3"/>
-      <c r="D109" s="5" t="s">
+      <c r="E110" s="18"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="23"/>
+      <c r="B111" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C111" s="11"/>
+      <c r="D111" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E109" s="10"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="9"/>
-      <c r="B110" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="C110" s="3"/>
-      <c r="D110" s="5" t="s">
+      <c r="E111" s="19"/>
+    </row>
+    <row r="112" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="23"/>
+      <c r="B112" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C112" s="11"/>
+      <c r="D112" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E110" s="10"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="9"/>
-      <c r="B111" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C111" s="3"/>
-      <c r="D111" s="5" t="s">
+      <c r="E112" s="20"/>
+    </row>
+    <row r="113" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="23"/>
+      <c r="B113" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C113" s="12"/>
+      <c r="D113" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="E111" s="10"/>
-    </row>
-    <row r="112" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A112" s="9"/>
-      <c r="B112" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C112" s="3"/>
-      <c r="D112" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E112" s="10"/>
-    </row>
-    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="9"/>
-      <c r="B113" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="C113" s="4"/>
-      <c r="D113" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E113" s="10"/>
+      <c r="E113" s="21"/>
     </row>
     <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="9"/>
+      <c r="A114" s="23"/>
       <c r="B114" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D114" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="E114" s="17"/>
+    </row>
+    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="23"/>
+      <c r="B115" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C115" s="11"/>
+      <c r="D115" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E115" s="18"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="23"/>
+      <c r="B116" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C116" s="11"/>
+      <c r="D116" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E114" s="10"/>
-    </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="9"/>
-      <c r="B115" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C115" s="3"/>
-      <c r="D115" s="5" t="s">
+      <c r="E116" s="19"/>
+    </row>
+    <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="23"/>
+      <c r="B117" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C117" s="11"/>
+      <c r="D117" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E115" s="10"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="9"/>
-      <c r="B116" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C116" s="3"/>
-      <c r="D116" s="5" t="s">
+      <c r="E117" s="20"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="23"/>
+      <c r="B118" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C118" s="11"/>
+      <c r="D118" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E116" s="10"/>
-    </row>
-    <row r="117" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="9"/>
-      <c r="B117" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="C117" s="3"/>
-      <c r="D117" s="5" t="s">
+      <c r="E118" s="20"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="23"/>
+      <c r="B119" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C119" s="11"/>
+      <c r="D119" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E117" s="10"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="9"/>
-      <c r="B118" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="C118" s="3"/>
-      <c r="D118" s="5" t="s">
+      <c r="E119" s="20"/>
+    </row>
+    <row r="120" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="23"/>
+      <c r="B120" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C120" s="12"/>
+      <c r="D120" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="E118" s="10"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="9"/>
-      <c r="B119" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="C119" s="3"/>
-      <c r="D119" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="E119" s="10"/>
-    </row>
-    <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="9"/>
-      <c r="B120" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C120" s="4"/>
-      <c r="D120" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="E120" s="10"/>
+      <c r="E120" s="21"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="9"/>
+      <c r="A121" s="23"/>
       <c r="B121" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D121" s="5" t="s">
+      <c r="D121" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="E121" s="2"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="23"/>
+      <c r="B122" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C122" s="11"/>
+      <c r="D122" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E122" s="3"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="23"/>
+      <c r="B123" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C123" s="11"/>
+      <c r="D123" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E121" s="10"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="9"/>
-      <c r="B122" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="C122" s="3"/>
-      <c r="D122" s="5" t="s">
+      <c r="E123" s="19"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="23"/>
+      <c r="B124" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C124" s="11"/>
+      <c r="D124" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E122" s="10"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="9"/>
-      <c r="B123" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="C123" s="3"/>
-      <c r="D123" s="5" t="s">
+      <c r="E124" s="20"/>
+    </row>
+    <row r="125" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="23"/>
+      <c r="B125" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C125" s="12"/>
+      <c r="D125" s="27" t="s">
         <v>255</v>
       </c>
-      <c r="E123" s="10"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="9"/>
-      <c r="B124" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C124" s="3"/>
-      <c r="D124" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="E124" s="10"/>
-    </row>
-    <row r="125" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="9"/>
-      <c r="B125" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="C125" s="4"/>
-      <c r="D125" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="E125" s="10"/>
+      <c r="E125" s="21"/>
     </row>
     <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126" s="9"/>
+      <c r="A126" s="23"/>
       <c r="B126" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D126" s="5" t="s">
+      <c r="D126" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="E126" s="17"/>
+    </row>
+    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A127" s="23"/>
+      <c r="B127" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C127" s="11"/>
+      <c r="D127" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E127" s="18"/>
+    </row>
+    <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A128" s="23"/>
+      <c r="B128" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C128" s="11"/>
+      <c r="D128" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E126" s="10"/>
-    </row>
-    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A127" s="9"/>
-      <c r="B127" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="C127" s="3"/>
-      <c r="D127" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E127" s="10"/>
-    </row>
-    <row r="128" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="9"/>
-      <c r="B128" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="C128" s="3"/>
-      <c r="D128" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="E128" s="10"/>
+      <c r="E128" s="19"/>
     </row>
     <row r="129" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="11"/>
+      <c r="A129" s="31"/>
       <c r="B129" s="26" t="s">
         <v>126</v>
       </c>
       <c r="C129" s="12"/>
-      <c r="D129" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="E129" s="13"/>
+      <c r="D129" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E129" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="C126:C129"/>
-    <mergeCell ref="C121:C125"/>
-    <mergeCell ref="C114:C120"/>
-    <mergeCell ref="C107:C113"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="C81:C86"/>
-    <mergeCell ref="C87:C93"/>
-    <mergeCell ref="C94:C100"/>
+  <mergeCells count="69">
+    <mergeCell ref="E123:E125"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="E111:E113"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="E116:E120"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="E91:E93"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="E98:E100"/>
+    <mergeCell ref="E101:E103"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="E76:E78"/>
+    <mergeCell ref="E81:E83"/>
+    <mergeCell ref="E84:E86"/>
+    <mergeCell ref="E87:E88"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="E63:E65"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="E70:E72"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E33:E37"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="C4:C11"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="A4:A24"/>
+    <mergeCell ref="A25:A50"/>
+    <mergeCell ref="A51:A75"/>
+    <mergeCell ref="A76:A103"/>
+    <mergeCell ref="A104:A129"/>
     <mergeCell ref="C101:C103"/>
     <mergeCell ref="C25:C28"/>
     <mergeCell ref="C29:C37"/>
@@ -3425,15 +3580,16 @@
     <mergeCell ref="C63:C65"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="C51:C59"/>
-    <mergeCell ref="A4:A24"/>
-    <mergeCell ref="A25:A50"/>
-    <mergeCell ref="A51:A75"/>
-    <mergeCell ref="A76:A103"/>
-    <mergeCell ref="A104:A129"/>
-    <mergeCell ref="C4:C11"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C76:C80"/>
+    <mergeCell ref="C81:C86"/>
+    <mergeCell ref="C87:C93"/>
+    <mergeCell ref="C94:C100"/>
+    <mergeCell ref="C126:C129"/>
+    <mergeCell ref="C121:C125"/>
+    <mergeCell ref="C114:C120"/>
+    <mergeCell ref="C107:C113"/>
+    <mergeCell ref="C104:C106"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="http://www.corestandards.org/Math/Content/1/OA/A/1/"/>

</xml_diff>